<commit_message>
Added some comments and updated defect log.
</commit_message>
<xml_diff>
--- a/Defect Log.xlsx
+++ b/Defect Log.xlsx
@@ -5,21 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jematanevar\Documents\New Data Rep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jematanevar\OneDrive - University of Texas at El Paso\Documents\Data Rep - Deploy\Data Repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21702D29-99CB-4C3A-B0E7-EC8227D6D954}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{21702D29-99CB-4C3A-B0E7-EC8227D6D954}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{18EB5775-35F3-4915-BCC0-8CA4C5A03F04}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" firstSheet="1" activeTab="3" xr2:uid="{073DD6F3-CF00-412D-A626-9DE335390389}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="4" xr2:uid="{073DD6F3-CF00-412D-A626-9DE335390389}"/>
   </bookViews>
   <sheets>
-    <sheet name="Defect Log-Poverty" sheetId="5" r:id="rId1"/>
-    <sheet name="Defect Log-Population" sheetId="1" r:id="rId2"/>
-    <sheet name="Defect Log-Employment" sheetId="4" r:id="rId3"/>
-    <sheet name="Defect Log-Industry" sheetId="6" r:id="rId4"/>
-    <sheet name="Defect Log -Trade" sheetId="7" r:id="rId5"/>
-    <sheet name="Defect Types" sheetId="2" r:id="rId6"/>
-    <sheet name="Template" sheetId="3" r:id="rId7"/>
+    <sheet name="Dictionary" sheetId="12" r:id="rId1"/>
+    <sheet name="Defect Types" sheetId="2" r:id="rId2"/>
+    <sheet name="Defect Log-Poverty" sheetId="5" r:id="rId3"/>
+    <sheet name="General Defect Log" sheetId="8" r:id="rId4"/>
+    <sheet name="Defect Log-Education" sheetId="9" r:id="rId5"/>
+    <sheet name="Defect Log-Population" sheetId="1" r:id="rId6"/>
+    <sheet name="Defect Log-Employment" sheetId="4" r:id="rId7"/>
+    <sheet name="Defect Log-Industry" sheetId="6" r:id="rId8"/>
+    <sheet name="Defect Log -Trade" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet6" sheetId="13" r:id="rId10"/>
+    <sheet name="Template" sheetId="3" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="97">
   <si>
     <t>Document/ Component Name</t>
   </si>
@@ -223,13 +227,112 @@
   </si>
   <si>
     <t xml:space="preserve">Dataset has two values for the same category. </t>
+  </si>
+  <si>
+    <t>Navigation Bar</t>
+  </si>
+  <si>
+    <t>General Review</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More space is needed between the nagivation bar and the rest of the elements. </t>
+  </si>
+  <si>
+    <t>Graph Legend</t>
+  </si>
+  <si>
+    <t>Legend title should let user know that they can select and isolate legend elements.</t>
+  </si>
+  <si>
+    <t>Information Box</t>
+  </si>
+  <si>
+    <t>The information box should be smaller or not bolded.</t>
+  </si>
+  <si>
+    <t>Pages space</t>
+  </si>
+  <si>
+    <t>For pages that have tabs, there should be more space between tabs and titles.</t>
+  </si>
+  <si>
+    <t>X axis slider</t>
+  </si>
+  <si>
+    <t>Some graphs are missing a title for the X axis slider.</t>
+  </si>
+  <si>
+    <t>X axis font weight</t>
+  </si>
+  <si>
+    <t>Labels for x axis should be bold.</t>
+  </si>
+  <si>
+    <t>Edit Button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Graph button should be aligned with dropdowns. </t>
+  </si>
+  <si>
+    <t>Compare buttons</t>
+  </si>
+  <si>
+    <t>The label for these buttons should say "Click to Compare"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Titles for gauges should be centered. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The content of gauges should be dark blue. </t>
+  </si>
+  <si>
+    <t>Main titles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main titles should have HR line below. </t>
+  </si>
+  <si>
+    <t>Data table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The font of the table should follow the font of the project. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The table should display percentages, not decimals of percentages. </t>
+  </si>
+  <si>
+    <t>The component being affected.</t>
+  </si>
+  <si>
+    <t>The type of deffect to fix. Refer to Defect Types</t>
+  </si>
+  <si>
+    <t>The moment at which the defect was injected.</t>
+  </si>
+  <si>
+    <t>The moment at which the defect was removed.</t>
+  </si>
+  <si>
+    <t>Rank of defect (Major or Minor)</t>
+  </si>
+  <si>
+    <t>The cost in minutes of fixing this defect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bief description of the defect. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend is shared, but when clicked glaph empties. This defect was added when there were two graphs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Although legend is shared, there seem to be inconsistencies with the colors. This defect was added when there were two graphs. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +340,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,8 +368,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -266,14 +383,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,6 +443,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{832B9013-8DE4-4D68-8BBD-5D3F39F52C62}" name="Table4" displayName="Table4" ref="A1:B1048576" totalsRowShown="0">
+  <autoFilter ref="A1:B1048576" xr:uid="{8AE70EF7-07DF-4B05-A91B-C3EB5C7EEB85}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{734F52C2-36A3-4BE8-9511-658D5772259F}" name="Type"/>
+    <tableColumn id="2" xr3:uid="{DC0331CF-B9DB-46B6-AC1F-F79A1534AB05}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{9A5BE84C-69A3-4F48-8AE0-B27E26341616}" name="Table326" displayName="Table326" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{55F234D9-12F9-4A39-9A0C-4D555293972E}"/>
   <tableColumns count="7">
@@ -307,7 +469,39 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0E9064A4-7D3C-4E70-94D4-820F9F2AA1DF}" name="Table329" displayName="Table329" ref="A1:G1048576" totalsRowShown="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{34C27068-B120-4970-8CB3-CAD2765BDF58}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{B99F5330-83F2-4C2A-9B81-E2BD3A84E99E}" name="Document/ Component Name"/>
+    <tableColumn id="2" xr3:uid="{0BFA2150-9947-4C57-9D42-655EFF130FCA}" name="Defect Type"/>
+    <tableColumn id="3" xr3:uid="{3A7DF0F4-0E2A-4EE5-A8DD-745964106B62}" name="Injection Phase"/>
+    <tableColumn id="4" xr3:uid="{60FEF6C4-BB74-4A6D-A62D-A5D025DDF54C}" name="Removal Phase"/>
+    <tableColumn id="5" xr3:uid="{7F5EC7F2-B22A-4CF6-8DE8-F8E347A4E020}" name="Major/Minor Defect"/>
+    <tableColumn id="6" xr3:uid="{740F7166-5FC5-4A9C-9C34-5727AF257DD9}" name="Fix Cost"/>
+    <tableColumn id="7" xr3:uid="{282411C6-C167-4D4C-BE2F-72B9857A6A77}" name="Defect Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FFC2D45B-3E06-43BD-AD30-3670B2C906EA}" name="Table3210" displayName="Table3210" ref="A1:G1048576" totalsRowShown="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{CFF395EF-3E10-478C-8E3D-1A178C669447}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{51E360A5-B85A-44FF-81D6-F2F9AC1A6D6A}" name="Document/ Component Name"/>
+    <tableColumn id="2" xr3:uid="{CCF65E39-23A3-4280-AE46-29FC94FEA7D3}" name="Defect Type"/>
+    <tableColumn id="3" xr3:uid="{71B47B21-F650-4362-BF11-1DF7ABEF167D}" name="Injection Phase"/>
+    <tableColumn id="4" xr3:uid="{F48BD0B9-4F4C-450D-9F74-71C04FB16566}" name="Removal Phase"/>
+    <tableColumn id="5" xr3:uid="{A528D04C-A990-41FD-BB7A-91F8A756BA4C}" name="Major/Minor Defect"/>
+    <tableColumn id="6" xr3:uid="{47F9B28B-713A-4C36-8BDE-95C60A96BD9A}" name="Fix Cost"/>
+    <tableColumn id="7" xr3:uid="{82838E11-3FB9-49B7-9CA1-3305028CA8CE}" name="Defect Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{93A1C920-07B6-472C-89A3-9E3DDA681CA3}" name="Table3" displayName="Table3" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{0275536E-BE03-4BFB-BA16-A7EF32570A0E}"/>
   <tableColumns count="7">
@@ -323,7 +517,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F12B541-B3A4-4728-8F2E-86CD24F7DCEC}" name="Table323" displayName="Table323" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{4D10988F-65DA-4DDA-B5D1-12467464ACB3}"/>
   <tableColumns count="7">
@@ -339,7 +533,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00B2FDF6-7D77-4F7A-AFD9-E2268EBEDE7B}" name="Table327" displayName="Table327" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{55F234D9-12F9-4A39-9A0C-4D555293972E}"/>
   <tableColumns count="7">
@@ -355,7 +549,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{25F08562-C092-47FF-A537-D8FB5B650080}" name="Table328" displayName="Table328" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{55F234D9-12F9-4A39-9A0C-4D555293972E}"/>
   <tableColumns count="7">
@@ -371,18 +565,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{832B9013-8DE4-4D68-8BBD-5D3F39F52C62}" name="Table4" displayName="Table4" ref="A1:B1048576" totalsRowShown="0">
-  <autoFilter ref="A1:B1048576" xr:uid="{8AE70EF7-07DF-4B05-A91B-C3EB5C7EEB85}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{734F52C2-36A3-4BE8-9511-658D5772259F}" name="Type"/>
-    <tableColumn id="2" xr3:uid="{DC0331CF-B9DB-46B6-AC1F-F79A1534AB05}" name="Description"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3DFA87C-32BD-4526-94EB-2AE75E4A8751}" name="Table32" displayName="Table32" ref="A1:G1048576" totalsRowShown="0">
   <autoFilter ref="A1:G1048576" xr:uid="{55F234D9-12F9-4A39-9A0C-4D555293972E}"/>
   <tableColumns count="7">
@@ -694,14 +877,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6CE13A-9B42-4AB0-A1C0-7EF14155A63A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38E945F5-3410-4F15-9663-AD9EB769B49E}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A97A73DE-6E18-4ACF-9DF4-B032032B621C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2177B6A2-FFB4-4777-9F52-A13AB6F79678}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,75 +1012,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -816,11 +1021,79 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A211B0E0-A880-4B36-9DEA-F47BBCC933CA}">
-  <dimension ref="A1:G15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7F56B0-AE89-4615-8DA8-2E5706FDCBAE}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA6CE13A-9B42-4AB0-A1C0-7EF14155A63A}">
+  <sheetPr>
+    <tabColor theme="9"/>
+  </sheetPr>
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,324 +1132,71 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="1">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1">
-        <v>15</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="1">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="1">
-        <v>2</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="1">
-        <v>20</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1">
-        <v>3</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="1">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="1">
-        <v>2</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="1">
-        <v>15</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1187,12 +1207,269 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA34E1DA-779E-4DB7-870B-22B924380FA2}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB1FB5E-1965-410D-89F3-52D783AD351A}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="76.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1">
+        <v>20</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="1">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129E7E24-8019-492E-BCA2-EC54018EE5B1}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,41 +1507,47 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
-        <v>56</v>
+      <c r="A2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1275,14 +1558,520 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A211B0E0-A880-4B36-9DEA-F47BBCC933CA}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="68.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1">
+        <v>5</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="1">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1">
+        <v>15</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1">
+        <v>10</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="1">
+        <v>20</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1">
+        <v>10</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="1">
+        <v>2</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="1">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA34E1DA-779E-4DB7-870B-22B924380FA2}">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="7" max="7" width="68.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28B38BBB-18C8-4D1B-B188-D9D53FEF44D4}">
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +2140,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C707795-8D3B-4EB3-8E3B-2271B771B422}">
   <sheetPr>
     <tabColor theme="9"/>
@@ -1469,119 +2258,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7F56B0-AE89-4615-8DA8-2E5706FDCBAE}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2177B6A2-FFB4-4777-9F52-A13AB6F79678}">
-  <sheetPr>
-    <tabColor theme="9"/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="68.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>